<commit_message>
Fix ETL + se sube API publica
</commit_message>
<xml_diff>
--- a/ETL/Version ETL/VS ETL 2024.xlsx
+++ b/ETL/Version ETL/VS ETL 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\3D Objects\Project-Dengue\ETL\Version ETL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D753911-A87E-4FB0-A967-314EB387FF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7837E0E3-574D-4BB0-BC1D-9BD7B018FAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
     <t>`1/1/2024`</t>
   </si>
   <si>
-    <t>`19/04/2024`</t>
+    <t>`31/12/2024`</t>
   </si>
 </sst>
 </file>
@@ -879,13 +879,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1269,7 +1265,7 @@
   <dimension ref="A1:N1274"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E2" sqref="E2:E1274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,47 +1281,47 @@
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>